<commit_message>
working on level 3 assignment 1
</commit_message>
<xml_diff>
--- a/UiPath/Training Course/Level 3/REFramework/ReFrameWork-master/ReFrameWork-master/Data/Config.xlsx
+++ b/UiPath/Training Course/Level 3/REFramework/ReFrameWork-master/ReFrameWork-master/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12450" windowHeight="4650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -170,16 +170,16 @@
     <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
   </si>
   <si>
-    <t>System1 URL</t>
-  </si>
-  <si>
-    <t>SHA1 Online URL</t>
+    <t>System1URL</t>
+  </si>
+  <si>
+    <t>SHA1OnlineURL</t>
+  </si>
+  <si>
+    <t>http://www.sha1-online.com/</t>
   </si>
   <si>
     <t>https://acme-test.uipath.com/account/login</t>
-  </si>
-  <si>
-    <t>http://www.sha1-online.com/</t>
   </si>
   <si>
     <t>System1_Credential</t>
@@ -189,7 +189,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -207,13 +207,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2D2F30"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -225,18 +237,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -517,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -592,15 +606,15 @@
         <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>50</v>
       </c>
-      <c r="B7" t="s">
-        <v>52</v>
+      <c r="B7" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1601,8 +1615,11 @@
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1610,8 +1627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1661,7 +1678,7 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">

</xml_diff>